<commit_message>
fix loadTabelInvestasi, banyak kegiatan per kriteria
</commit_message>
<xml_diff>
--- a/data/pekalongan.xlsx
+++ b/data/pekalongan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RIQQI\SERVER\htdocs\motorKawanku\motorkawanku\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291A4349-9929-44C0-889C-11F93D7EDA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEA319C-06F4-47DD-88D7-2AF2C24FEF1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{59B733E0-D555-495B-93A0-705B2FB4D176}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{59B733E0-D555-495B-93A0-705B2FB4D176}"/>
   </bookViews>
   <sheets>
     <sheet name="kota" sheetId="5" r:id="rId1"/>
@@ -77,21 +77,12 @@
     <t>b. Kepadatan Bangunan</t>
   </si>
   <si>
-    <t>c. Ketidaksesuaian dengan Persy Teknis Bangunan</t>
-  </si>
-  <si>
     <t>a. Cakupan Pelayanan Jalan Lingkungan</t>
   </si>
   <si>
-    <t>b. Kualitas Permukaan Jalan lingkungan</t>
-  </si>
-  <si>
     <t>a. Ketersediaan Akses Aman Air Minum</t>
   </si>
   <si>
-    <t>b. Tidak terpenuhinya Kebutuhan Air Minum</t>
-  </si>
-  <si>
     <t>a. Ketidakmampuan Mengalirkan Limpasan Air</t>
   </si>
   <si>
@@ -101,15 +92,6 @@
     <t>a. Sistem Pengelolaan Air Limbah Tidak Sesuai Standar Teknis</t>
   </si>
   <si>
-    <t>b. Prasarana dan Sarana Pengelolaan Air Limbah Tidak Sesuai dengan Persyaratan Teknis</t>
-  </si>
-  <si>
-    <t>a. Prasarana dan Sarana Persampahan Tidak Sesuai dengan persyaratan Teknis</t>
-  </si>
-  <si>
-    <t>b. Sistem Pengelolaan Persampahan yang tidak sesuai Standar Teknis</t>
-  </si>
-  <si>
     <t>a. Ketidaktersediaan Prasarana Proteksi Kebakaran</t>
   </si>
   <si>
@@ -203,28 +185,7 @@
     <t>ket</t>
   </si>
   <si>
-    <t>kondisi bangunan gedung</t>
-  </si>
-  <si>
     <t>aspek</t>
-  </si>
-  <si>
-    <t>kondisi jalan lingkungan</t>
-  </si>
-  <si>
-    <t>kondisi penyediaan air minum</t>
-  </si>
-  <si>
-    <t>kondisi drainase lingkungan</t>
-  </si>
-  <si>
-    <t>kondisi pengelolaan air limbah</t>
-  </si>
-  <si>
-    <t>kondisi pengelolaan persampahan</t>
-  </si>
-  <si>
-    <t>kondisi proteksi kebakaran</t>
   </si>
   <si>
     <t>rata-rata</t>
@@ -269,9 +230,6 @@
     <t>c. Kualitas Konstruksi Drainase</t>
   </si>
   <si>
-    <t>a. ketidakteraturan bangunan</t>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
@@ -456,6 +414,48 @@
   </si>
   <si>
     <t>kontribusiPenanganan</t>
+  </si>
+  <si>
+    <t>1. Kondisi Bangunan Gedung</t>
+  </si>
+  <si>
+    <t>2. Kondisi Jalan Lingkungan</t>
+  </si>
+  <si>
+    <t>3. Kondisi Penyediaan Air Minum</t>
+  </si>
+  <si>
+    <t>4. Kondisi Drainase Lingkungan</t>
+  </si>
+  <si>
+    <t>5. Kondisi Pengelolaan Air Limbah</t>
+  </si>
+  <si>
+    <t>6. Kondisi Pengelolaan Persampahan</t>
+  </si>
+  <si>
+    <t>7. Kondisi Proteksi Kebakaran</t>
+  </si>
+  <si>
+    <t>a. Ketidakteraturan Bangunan</t>
+  </si>
+  <si>
+    <t>c. Ketidaksesuaian Dengan Persy Teknis Bangunan</t>
+  </si>
+  <si>
+    <t>b. Kualitas Permukaan Jalan Lingkungan</t>
+  </si>
+  <si>
+    <t>b. Tidak Terpenuhinya Kebutuhan Air Minum</t>
+  </si>
+  <si>
+    <t>b. Prasarana Dan Sarana Pengelolaan Air Limbah Tidak Sesuai Dengan Persyaratan Teknis</t>
+  </si>
+  <si>
+    <t>a. Prasarana Dan Sarana Persampahan Tidak Sesuai Dengan Persyaratan Teknis</t>
+  </si>
+  <si>
+    <t>b. Sistem Pengelolaan Persampahan Yang Tidak Sesuai Standar Teknis</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,6 +477,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -514,10 +521,13 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma 2" xfId="3" xr:uid="{4188CA50-A9B7-4441-A52F-DE73B0767E71}"/>
@@ -1117,19 +1127,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1137,16 +1147,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1174,31 +1184,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="F1" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="G1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="H1" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="I1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1206,10 +1216,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>8</v>
@@ -1255,28 +1265,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="E1" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="F1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="G1" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="H1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1287,7 +1297,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>0.84880800000000001</v>
@@ -1313,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>1.104724</v>
@@ -1339,7 +1349,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>1.7053769999999999</v>
@@ -1365,7 +1375,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>1.1329070000000001</v>
@@ -1391,7 +1401,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>1.2737909999999999</v>
@@ -1417,7 +1427,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>1.8216680000000001</v>
@@ -1443,7 +1453,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D8">
         <v>2.4502660000000001</v>
@@ -1469,7 +1479,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D9">
         <v>1.2417579999999999</v>
@@ -1557,190 +1567,190 @@
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
-      </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" t="s">
+        <v>88</v>
+      </c>
+      <c r="O1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>89</v>
+      </c>
+      <c r="R1" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" t="s">
+        <v>90</v>
+      </c>
+      <c r="V1" t="s">
+        <v>63</v>
+      </c>
+      <c r="W1" t="s">
+        <v>64</v>
+      </c>
+      <c r="X1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK1" t="s">
         <v>59</v>
       </c>
-      <c r="H1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J1" t="s">
-        <v>101</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="AL1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BF1" t="s">
         <v>68</v>
       </c>
-      <c r="L1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N1" t="s">
-        <v>102</v>
-      </c>
-      <c r="O1" t="s">
-        <v>71</v>
-      </c>
-      <c r="P1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>103</v>
-      </c>
-      <c r="R1" t="s">
-        <v>74</v>
-      </c>
-      <c r="S1" t="s">
-        <v>75</v>
-      </c>
-      <c r="T1" t="s">
-        <v>67</v>
-      </c>
-      <c r="U1" t="s">
-        <v>104</v>
-      </c>
-      <c r="V1" t="s">
-        <v>77</v>
-      </c>
-      <c r="W1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X1" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AL1" t="s">
+      <c r="BG1" t="s">
         <v>109</v>
       </c>
-      <c r="AM1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AO1" t="s">
+      <c r="BH1" t="s">
         <v>110</v>
       </c>
-      <c r="AP1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AS1" t="s">
+      <c r="BI1" t="s">
         <v>111</v>
       </c>
-      <c r="AT1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AV1" t="s">
+      <c r="BJ1" t="s">
         <v>112</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>113</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>97</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>98</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>114</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>100</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>82</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>123</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>124</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>125</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.25">
@@ -1922,7 +1932,7 @@
         <v>16</v>
       </c>
       <c r="BH2" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="BI2">
         <v>0.22675162072980901</v>
@@ -1942,8 +1952,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:BJ42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AN26" sqref="AN26"/>
+    <sheetView topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC16" sqref="AC16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,190 +1994,190 @@
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" t="s">
+        <v>88</v>
+      </c>
+      <c r="O1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>89</v>
+      </c>
+      <c r="R1" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" t="s">
+        <v>90</v>
+      </c>
+      <c r="V1" t="s">
+        <v>63</v>
+      </c>
+      <c r="W1" t="s">
+        <v>64</v>
+      </c>
+      <c r="X1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK1" t="s">
         <v>59</v>
       </c>
-      <c r="H1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J1" t="s">
-        <v>101</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="AL1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BF1" t="s">
         <v>68</v>
       </c>
-      <c r="L1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N1" t="s">
-        <v>102</v>
-      </c>
-      <c r="O1" t="s">
-        <v>71</v>
-      </c>
-      <c r="P1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>103</v>
-      </c>
-      <c r="R1" t="s">
-        <v>74</v>
-      </c>
-      <c r="S1" t="s">
-        <v>75</v>
-      </c>
-      <c r="T1" t="s">
-        <v>67</v>
-      </c>
-      <c r="U1" t="s">
-        <v>104</v>
-      </c>
-      <c r="V1" t="s">
-        <v>77</v>
-      </c>
-      <c r="W1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X1" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AL1" t="s">
+      <c r="BG1" t="s">
         <v>109</v>
       </c>
-      <c r="AM1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AO1" t="s">
+      <c r="BH1" t="s">
         <v>110</v>
       </c>
-      <c r="AP1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AS1" t="s">
+      <c r="BI1" t="s">
         <v>111</v>
       </c>
-      <c r="AT1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AV1" t="s">
+      <c r="BJ1" t="s">
         <v>112</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>113</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>97</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>98</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>114</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>100</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>82</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>123</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>124</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>125</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.25">
@@ -2349,7 +2359,7 @@
         <v>19</v>
       </c>
       <c r="BH2" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="BI2">
         <v>0.24460317460317457</v>
@@ -2537,7 +2547,7 @@
         <v>18</v>
       </c>
       <c r="BH3" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="BI3">
         <v>0.20619282195636873</v>
@@ -2725,7 +2735,7 @@
         <v>16</v>
       </c>
       <c r="BH4" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="BI4">
         <v>0.20764119601328904</v>
@@ -2913,7 +2923,7 @@
         <v>22</v>
       </c>
       <c r="BH5" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="BI5">
         <v>0.31194704175761007</v>
@@ -3101,7 +3111,7 @@
         <v>23</v>
       </c>
       <c r="BH6" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="BI6">
         <v>0.32470355731225303</v>
@@ -3289,7 +3299,7 @@
         <v>22</v>
       </c>
       <c r="BH7" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="BI7">
         <v>0.28693031118421208</v>
@@ -3477,7 +3487,7 @@
         <v>17</v>
       </c>
       <c r="BH8" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="BI8">
         <v>0.22004975736639551</v>
@@ -3665,7 +3675,7 @@
         <v>18</v>
       </c>
       <c r="BH9" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="BI9">
         <v>0.27636197336077289</v>
@@ -3690,8 +3700,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3711,82 +3721,84 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="J1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
         <v>41</v>
-      </c>
-      <c r="L1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" t="str">
+        <f>CONCATENATE(J2,K2)</f>
+        <v>1a</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="M2" t="s">
         <v>43</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>55</v>
-      </c>
-      <c r="L2" t="s">
-        <v>64</v>
-      </c>
-      <c r="M2" t="s">
-        <v>56</v>
-      </c>
       <c r="N2" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
+      <c r="B3" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I17" si="0">CONCATENATE(J3,K3)</f>
+        <v>1b</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3794,236 +3806,244 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
+      <c r="B4" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>1c</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>65</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
+      <c r="B5" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>2a</v>
       </c>
       <c r="J5">
         <v>2</v>
       </c>
       <c r="K5" t="s">
-        <v>55</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>2</v>
+        <v>42</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I6">
-        <v>5</v>
+      <c r="B6" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>2b</v>
       </c>
       <c r="J6">
         <v>2</v>
       </c>
       <c r="K6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>3</v>
+        <v>49</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7">
-        <v>6</v>
+      <c r="B7" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>3a</v>
       </c>
       <c r="J7">
         <v>3</v>
       </c>
       <c r="K7" t="s">
-        <v>55</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>4</v>
+        <v>42</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8">
-        <v>7</v>
+      <c r="B8" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>3b</v>
       </c>
       <c r="J8">
         <v>3</v>
       </c>
       <c r="K8" t="s">
-        <v>62</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>5</v>
+        <v>49</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I9">
-        <v>8</v>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>4a</v>
       </c>
       <c r="J9">
         <v>4</v>
       </c>
       <c r="K9" t="s">
-        <v>55</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>6</v>
+        <v>42</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I10">
-        <v>9</v>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>4b</v>
       </c>
       <c r="J10">
         <v>4</v>
       </c>
       <c r="K10" t="s">
-        <v>62</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>7</v>
+        <v>49</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I11">
-        <v>10</v>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>4c</v>
       </c>
       <c r="J11">
         <v>4</v>
       </c>
       <c r="K11" t="s">
-        <v>65</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>63</v>
+        <v>51</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I12">
-        <v>11</v>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>5a</v>
       </c>
       <c r="J12">
         <v>5</v>
       </c>
       <c r="K12" t="s">
-        <v>55</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>8</v>
+        <v>42</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I13">
-        <v>12</v>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>5b</v>
       </c>
       <c r="J13">
         <v>5</v>
       </c>
       <c r="K13" t="s">
-        <v>62</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>9</v>
+        <v>49</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I14">
-        <v>13</v>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>6a</v>
       </c>
       <c r="J14">
         <v>6</v>
       </c>
       <c r="K14" t="s">
-        <v>55</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>10</v>
+        <v>42</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I15">
-        <v>14</v>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>6b</v>
       </c>
       <c r="J15">
         <v>6</v>
       </c>
       <c r="K15" t="s">
-        <v>62</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>11</v>
+        <v>49</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I16">
-        <v>15</v>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>7a</v>
       </c>
       <c r="J16">
         <v>7</v>
       </c>
       <c r="K16" t="s">
-        <v>55</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I17">
-        <v>16</v>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>7b</v>
       </c>
       <c r="J17">
         <v>7</v>
       </c>
       <c r="K17" t="s">
-        <v>62</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>13</v>
+        <v>49</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="9:12" x14ac:dyDescent="0.25">
       <c r="L18" s="1"/>
-    </row>
-    <row r="19" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L19" t="e">
-        <f>TRANSPOSE(kumuhKawasan!I8:K23)</f>
-        <v>#VALUE!</v>
-      </c>
     </row>
     <row r="21" spans="9:12" x14ac:dyDescent="0.25">
       <c r="L21" s="1"/>

</xml_diff>

<commit_message>
adding tampilan kumuh awal & akhir (blom rumus)
</commit_message>
<xml_diff>
--- a/data/pekalongan.xlsx
+++ b/data/pekalongan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RIQQI\SERVER\htdocs\motorKawanku\motorkawanku\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEA319C-06F4-47DD-88D7-2AF2C24FEF1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A8AAE3-55B0-44E1-9DA6-4716655B7BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{59B733E0-D555-495B-93A0-705B2FB4D176}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="5" xr2:uid="{59B733E0-D555-495B-93A0-705B2FB4D176}"/>
   </bookViews>
   <sheets>
     <sheet name="kota" sheetId="5" r:id="rId1"/>
@@ -3698,10 +3698,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1A1EEB-957A-4E1B-9E65-ADA1598904B4}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="E1" sqref="E1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3709,17 +3709,16 @@
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="6.5703125" customWidth="1"/>
-    <col min="9" max="9" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="80.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="82.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="82.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -3729,326 +3728,327 @@
       <c r="C1" t="s">
         <v>38</v>
       </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
       <c r="I1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="J1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="I2" t="str">
-        <f>CONCATENATE(J2,K2)</f>
+      <c r="E2" t="str">
+        <f>CONCATENATE(F2,G2)</f>
         <v>1a</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>42</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="M2" t="s">
+      <c r="I2" t="s">
         <v>43</v>
       </c>
-      <c r="N2" t="s">
+      <c r="J2" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="I3" t="str">
-        <f t="shared" ref="I3:I17" si="0">CONCATENATE(J3,K3)</f>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E17" si="0">CONCATENATE(F3,G3)</f>
         <v>1b</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>49</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="I4" t="str">
+      <c r="E4" t="str">
         <f t="shared" si="0"/>
         <v>1c</v>
       </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>51</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="I5" t="str">
+      <c r="E5" t="str">
         <f t="shared" si="0"/>
         <v>2a</v>
       </c>
-      <c r="J5">
+      <c r="F5">
         <v>2</v>
       </c>
-      <c r="K5" t="s">
+      <c r="G5" t="s">
         <v>42</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H5" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="I6" t="str">
+      <c r="E6" t="str">
         <f t="shared" si="0"/>
         <v>2b</v>
       </c>
-      <c r="J6">
+      <c r="F6">
         <v>2</v>
       </c>
-      <c r="K6" t="s">
+      <c r="G6" t="s">
         <v>49</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="I7" t="str">
+      <c r="E7" t="str">
         <f t="shared" si="0"/>
         <v>3a</v>
       </c>
-      <c r="J7">
+      <c r="F7">
         <v>3</v>
       </c>
-      <c r="K7" t="s">
+      <c r="G7" t="s">
         <v>42</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="I8" t="str">
+      <c r="E8" t="str">
         <f t="shared" si="0"/>
         <v>3b</v>
       </c>
-      <c r="J8">
+      <c r="F8">
         <v>3</v>
       </c>
-      <c r="K8" t="s">
+      <c r="G8" t="s">
         <v>49</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I9" t="str">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E9" t="str">
         <f t="shared" si="0"/>
         <v>4a</v>
       </c>
-      <c r="J9">
+      <c r="F9">
         <v>4</v>
       </c>
-      <c r="K9" t="s">
+      <c r="G9" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I10" t="str">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E10" t="str">
         <f t="shared" si="0"/>
         <v>4b</v>
       </c>
-      <c r="J10">
+      <c r="F10">
         <v>4</v>
       </c>
-      <c r="K10" t="s">
+      <c r="G10" t="s">
         <v>49</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I11" t="str">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E11" t="str">
         <f t="shared" si="0"/>
         <v>4c</v>
       </c>
-      <c r="J11">
+      <c r="F11">
         <v>4</v>
       </c>
-      <c r="K11" t="s">
+      <c r="G11" t="s">
         <v>51</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I12" t="str">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E12" t="str">
         <f t="shared" si="0"/>
         <v>5a</v>
       </c>
-      <c r="J12">
+      <c r="F12">
         <v>5</v>
       </c>
-      <c r="K12" t="s">
+      <c r="G12" t="s">
         <v>42</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I13" t="str">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E13" t="str">
         <f t="shared" si="0"/>
         <v>5b</v>
       </c>
-      <c r="J13">
+      <c r="F13">
         <v>5</v>
       </c>
-      <c r="K13" t="s">
+      <c r="G13" t="s">
         <v>49</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I14" t="str">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E14" t="str">
         <f t="shared" si="0"/>
         <v>6a</v>
       </c>
-      <c r="J14">
+      <c r="F14">
         <v>6</v>
       </c>
-      <c r="K14" t="s">
+      <c r="G14" t="s">
         <v>42</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I15" t="str">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E15" t="str">
         <f t="shared" si="0"/>
         <v>6b</v>
       </c>
-      <c r="J15">
+      <c r="F15">
         <v>6</v>
       </c>
-      <c r="K15" t="s">
+      <c r="G15" t="s">
         <v>49</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I16" t="str">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E16" t="str">
         <f t="shared" si="0"/>
         <v>7a</v>
       </c>
-      <c r="J16">
+      <c r="F16">
         <v>7</v>
       </c>
-      <c r="K16" t="s">
+      <c r="G16" t="s">
         <v>42</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I17" t="str">
+    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E17" t="str">
         <f t="shared" si="0"/>
         <v>7b</v>
       </c>
-      <c r="J17">
+      <c r="F17">
         <v>7</v>
       </c>
-      <c r="K17" t="s">
+      <c r="G17" t="s">
         <v>49</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L18" s="1"/>
-    </row>
-    <row r="21" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L21" s="1"/>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding leaflet js, ( belum menyesuaikan rt)
</commit_message>
<xml_diff>
--- a/data/pekalongan.xlsx
+++ b/data/pekalongan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RIQQI\SERVER\htdocs\motorKawanku\motorkawanku\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08517807-DB9E-4C45-ABBA-807D1ED38F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE7D8FF-EF20-41E5-8710-1A594A5EEFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{59B733E0-D555-495B-93A0-705B2FB4D176}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{59B733E0-D555-495B-93A0-705B2FB4D176}"/>
   </bookViews>
   <sheets>
     <sheet name="kota" sheetId="5" r:id="rId1"/>
@@ -1319,7 +1319,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2076,8 +2076,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:BJ42"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC9" sqref="AC9"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AG32" sqref="AG32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3824,8 +3824,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3835,7 +3835,7 @@
     <col min="4" max="4" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="80.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
@@ -4172,116 +4172,208 @@
       <c r="F19" t="s">
         <v>129</v>
       </c>
+      <c r="G19" t="str">
+        <f>CONCATENATE("'",F19,"',")</f>
+        <v>'1a',</v>
+      </c>
     </row>
     <row r="20" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>130</v>
       </c>
+      <c r="G20" t="str">
+        <f t="shared" ref="G20:G41" si="1">CONCATENATE("'",F20,"',")</f>
+        <v>'1b',</v>
+      </c>
     </row>
     <row r="21" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
         <v>131</v>
       </c>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v>'1c',</v>
+      </c>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>52</v>
       </c>
+      <c r="G22" t="str">
+        <f t="shared" si="1"/>
+        <v>'1r',</v>
+      </c>
     </row>
     <row r="23" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
         <v>132</v>
       </c>
+      <c r="G23" t="str">
+        <f t="shared" si="1"/>
+        <v>'2a',</v>
+      </c>
     </row>
     <row r="24" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
         <v>133</v>
       </c>
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
+        <v>'2b',</v>
+      </c>
     </row>
     <row r="25" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
         <v>53</v>
       </c>
+      <c r="G25" t="str">
+        <f t="shared" si="1"/>
+        <v>'2r',</v>
+      </c>
     </row>
     <row r="26" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
         <v>134</v>
       </c>
+      <c r="G26" t="str">
+        <f t="shared" si="1"/>
+        <v>'3a',</v>
+      </c>
     </row>
     <row r="27" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>135</v>
       </c>
+      <c r="G27" t="str">
+        <f t="shared" si="1"/>
+        <v>'3b',</v>
+      </c>
     </row>
     <row r="28" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
         <v>56</v>
       </c>
+      <c r="G28" t="str">
+        <f t="shared" si="1"/>
+        <v>'3r',</v>
+      </c>
     </row>
     <row r="29" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
         <v>136</v>
       </c>
+      <c r="G29" t="str">
+        <f t="shared" si="1"/>
+        <v>'4a',</v>
+      </c>
     </row>
     <row r="30" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
         <v>137</v>
       </c>
+      <c r="G30" t="str">
+        <f t="shared" si="1"/>
+        <v>'4b',</v>
+      </c>
     </row>
     <row r="31" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
         <v>138</v>
       </c>
+      <c r="G31" t="str">
+        <f t="shared" si="1"/>
+        <v>'4c',</v>
+      </c>
     </row>
     <row r="32" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="G32" t="str">
+        <f t="shared" si="1"/>
+        <v>'4r',</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="G33" t="str">
+        <f t="shared" si="1"/>
+        <v>'5a',</v>
+      </c>
+    </row>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="G34" t="str">
+        <f t="shared" si="1"/>
+        <v>'5b',</v>
+      </c>
+    </row>
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="G35" t="str">
+        <f t="shared" si="1"/>
+        <v>'5r',</v>
+      </c>
+    </row>
+    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="G36" t="str">
+        <f t="shared" si="1"/>
+        <v>'6a',</v>
+      </c>
+    </row>
+    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="G37" t="str">
+        <f t="shared" si="1"/>
+        <v>'6b',</v>
+      </c>
+    </row>
+    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="G38" t="str">
+        <f t="shared" si="1"/>
+        <v>'6r',</v>
+      </c>
+    </row>
+    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F39" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="G39" t="str">
+        <f t="shared" si="1"/>
+        <v>'7a',</v>
+      </c>
+    </row>
+    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="41" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="G40" t="str">
+        <f t="shared" si="1"/>
+        <v>'7b',</v>
+      </c>
+    </row>
+    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F41" t="s">
         <v>68</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="1"/>
+        <v>'7r',</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing leaflet js adding polygon per kumuh kawasan / rt
</commit_message>
<xml_diff>
--- a/data/pekalongan.xlsx
+++ b/data/pekalongan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RIQQI\SERVER\htdocs\motorKawanku\motorkawanku\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE7D8FF-EF20-41E5-8710-1A594A5EEFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD39298-549C-4F5E-B1B8-9165A7423FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{59B733E0-D555-495B-93A0-705B2FB4D176}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{59B733E0-D555-495B-93A0-705B2FB4D176}"/>
   </bookViews>
   <sheets>
     <sheet name="kota" sheetId="5" r:id="rId1"/>
@@ -161,9 +161,6 @@
     <t>rt-rw</t>
   </si>
   <si>
-    <t>podosugih</t>
-  </si>
-  <si>
     <t>pekalongan barat</t>
   </si>
   <si>
@@ -510,6 +507,9 @@
   </si>
   <si>
     <t>7b</t>
+  </si>
+  <si>
+    <t>Podosugih</t>
   </si>
 </sst>
 </file>
@@ -1223,8 +1223,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,25 +1252,25 @@
         <v>28</v>
       </c>
       <c r="E1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" t="s">
         <v>104</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>105</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>106</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>107</v>
       </c>
-      <c r="I1" t="s">
-        <v>108</v>
-      </c>
       <c r="J1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K1" t="s">
         <v>127</v>
-      </c>
-      <c r="K1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1278,10 +1278,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" t="s">
         <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
       </c>
       <c r="D2">
         <v>8</v>
@@ -1341,28 +1341,28 @@
         <v>26</v>
       </c>
       <c r="C1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" t="s">
         <v>103</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>104</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>105</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>106</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>107</v>
       </c>
-      <c r="H1" t="s">
-        <v>108</v>
-      </c>
       <c r="I1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J1" t="s">
         <v>127</v>
-      </c>
-      <c r="J1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1697,184 +1697,184 @@
         <v>26</v>
       </c>
       <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
       <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" t="s">
-        <v>48</v>
-      </c>
       <c r="J1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" t="s">
         <v>87</v>
       </c>
-      <c r="K1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>88</v>
+      </c>
+      <c r="R1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S1" t="s">
+        <v>60</v>
+      </c>
+      <c r="T1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U1" t="s">
+        <v>89</v>
+      </c>
+      <c r="V1" t="s">
+        <v>62</v>
+      </c>
+      <c r="W1" t="s">
+        <v>63</v>
+      </c>
+      <c r="X1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA1" t="s">
         <v>55</v>
       </c>
-      <c r="M1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N1" t="s">
-        <v>88</v>
-      </c>
-      <c r="O1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="AB1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AK1" t="s">
         <v>58</v>
       </c>
-      <c r="Q1" t="s">
-        <v>89</v>
-      </c>
-      <c r="R1" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="AL1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR1" t="s">
         <v>61</v>
       </c>
-      <c r="T1" t="s">
-        <v>53</v>
-      </c>
-      <c r="U1" t="s">
-        <v>90</v>
-      </c>
-      <c r="V1" t="s">
-        <v>63</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="AS1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AY1" t="s">
         <v>64</v>
       </c>
-      <c r="X1" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z1" t="s">
+      <c r="AZ1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BF1" t="s">
         <v>67</v>
       </c>
-      <c r="AA1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>83</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>84</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>100</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>85</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>86</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>68</v>
-      </c>
       <c r="BG1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BH1" t="s">
         <v>109</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>110</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>111</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.25">
@@ -2056,7 +2056,7 @@
         <v>16</v>
       </c>
       <c r="BH2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI2">
         <v>0.22675162072980901</v>
@@ -2076,7 +2076,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:BJ42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AG32" sqref="AG32"/>
     </sheetView>
   </sheetViews>
@@ -2121,187 +2121,187 @@
         <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
       <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" t="s">
-        <v>48</v>
-      </c>
       <c r="J1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" t="s">
         <v>87</v>
       </c>
-      <c r="K1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>88</v>
+      </c>
+      <c r="R1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S1" t="s">
+        <v>60</v>
+      </c>
+      <c r="T1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U1" t="s">
+        <v>89</v>
+      </c>
+      <c r="V1" t="s">
+        <v>62</v>
+      </c>
+      <c r="W1" t="s">
+        <v>63</v>
+      </c>
+      <c r="X1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA1" t="s">
         <v>55</v>
       </c>
-      <c r="M1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N1" t="s">
-        <v>88</v>
-      </c>
-      <c r="O1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="AB1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AK1" t="s">
         <v>58</v>
       </c>
-      <c r="Q1" t="s">
-        <v>89</v>
-      </c>
-      <c r="R1" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="AL1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR1" t="s">
         <v>61</v>
       </c>
-      <c r="T1" t="s">
-        <v>53</v>
-      </c>
-      <c r="U1" t="s">
-        <v>90</v>
-      </c>
-      <c r="V1" t="s">
-        <v>63</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="AS1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AY1" t="s">
         <v>64</v>
       </c>
-      <c r="X1" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z1" t="s">
+      <c r="AZ1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BF1" t="s">
         <v>67</v>
       </c>
-      <c r="AA1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>83</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>84</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>100</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>85</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>86</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>68</v>
-      </c>
       <c r="BG1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BH1" t="s">
         <v>109</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>110</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>111</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.25">
@@ -2483,7 +2483,7 @@
         <v>19</v>
       </c>
       <c r="BH2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI2">
         <v>0.24460317460317457</v>
@@ -2671,7 +2671,7 @@
         <v>18</v>
       </c>
       <c r="BH3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI3">
         <v>0.20619282195636873</v>
@@ -2859,7 +2859,7 @@
         <v>16</v>
       </c>
       <c r="BH4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI4">
         <v>0.20764119601328904</v>
@@ -3047,7 +3047,7 @@
         <v>22</v>
       </c>
       <c r="BH5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI5">
         <v>0.31194704175761007</v>
@@ -3235,7 +3235,7 @@
         <v>23</v>
       </c>
       <c r="BH6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI6">
         <v>0.32470355731225303</v>
@@ -3423,7 +3423,7 @@
         <v>22</v>
       </c>
       <c r="BH7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI7">
         <v>0.28693031118421208</v>
@@ -3611,7 +3611,7 @@
         <v>17</v>
       </c>
       <c r="BH8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI8">
         <v>0.22004975736639551</v>
@@ -3799,7 +3799,7 @@
         <v>18</v>
       </c>
       <c r="BH9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI9">
         <v>0.27636197336077289</v>
@@ -3844,34 +3844,34 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
       </c>
       <c r="E1" t="s">
         <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
       <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
         <v>39</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>40</v>
-      </c>
-      <c r="K1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3879,7 +3879,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E2" t="str">
         <f>CONCATENATE(F2,G2)</f>
@@ -3889,19 +3889,19 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>43</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -3909,7 +3909,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E17" si="0">CONCATENATE(F3,G3)</f>
@@ -3919,7 +3919,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>0</v>
@@ -3930,7 +3930,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -3940,10 +3940,10 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3951,7 +3951,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -3961,7 +3961,7 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>1</v>
@@ -3972,7 +3972,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -3982,10 +3982,10 @@
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3993,7 +3993,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -4003,7 +4003,7 @@
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>2</v>
@@ -4014,7 +4014,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -4024,10 +4024,10 @@
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -4039,7 +4039,7 @@
         <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>3</v>
@@ -4054,7 +4054,7 @@
         <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>4</v>
@@ -4069,10 +4069,10 @@
         <v>4</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -4084,7 +4084,7 @@
         <v>5</v>
       </c>
       <c r="G12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>5</v>
@@ -4099,10 +4099,10 @@
         <v>5</v>
       </c>
       <c r="G13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -4114,10 +4114,10 @@
         <v>6</v>
       </c>
       <c r="G14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -4129,10 +4129,10 @@
         <v>6</v>
       </c>
       <c r="G15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -4144,7 +4144,7 @@
         <v>7</v>
       </c>
       <c r="G16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>6</v>
@@ -4159,7 +4159,7 @@
         <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>7</v>
@@ -4170,7 +4170,7 @@
     </row>
     <row r="19" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G19" t="str">
         <f>CONCATENATE("'",F19,"',")</f>
@@ -4179,7 +4179,7 @@
     </row>
     <row r="20" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" ref="G20:G41" si="1">CONCATENATE("'",F20,"',")</f>
@@ -4188,7 +4188,7 @@
     </row>
     <row r="21" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="1"/>
@@ -4198,7 +4198,7 @@
     </row>
     <row r="22" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="1"/>
@@ -4207,7 +4207,7 @@
     </row>
     <row r="23" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
@@ -4216,7 +4216,7 @@
     </row>
     <row r="24" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="1"/>
@@ -4225,7 +4225,7 @@
     </row>
     <row r="25" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="1"/>
@@ -4234,7 +4234,7 @@
     </row>
     <row r="26" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="1"/>
@@ -4243,7 +4243,7 @@
     </row>
     <row r="27" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="1"/>
@@ -4252,7 +4252,7 @@
     </row>
     <row r="28" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="1"/>
@@ -4261,7 +4261,7 @@
     </row>
     <row r="29" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="1"/>
@@ -4270,7 +4270,7 @@
     </row>
     <row r="30" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="1"/>
@@ -4279,7 +4279,7 @@
     </row>
     <row r="31" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="1"/>
@@ -4288,7 +4288,7 @@
     </row>
     <row r="32" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="1"/>
@@ -4297,7 +4297,7 @@
     </row>
     <row r="33" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="1"/>
@@ -4306,7 +4306,7 @@
     </row>
     <row r="34" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="1"/>
@@ -4315,7 +4315,7 @@
     </row>
     <row r="35" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="1"/>
@@ -4324,7 +4324,7 @@
     </row>
     <row r="36" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="1"/>
@@ -4333,7 +4333,7 @@
     </row>
     <row r="37" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="1"/>
@@ -4342,7 +4342,7 @@
     </row>
     <row r="38" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="1"/>
@@ -4351,7 +4351,7 @@
     </row>
     <row r="39" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="1"/>
@@ -4360,7 +4360,7 @@
     </row>
     <row r="40" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="1"/>
@@ -4369,7 +4369,7 @@
     </row>
     <row r="41" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
mengubah tampilan baseline menjadi react
</commit_message>
<xml_diff>
--- a/data/pekalongan.xlsx
+++ b/data/pekalongan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RIQQI\SERVER\htdocs\motorKawanku\motorkawanku\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7C3425-A467-4935-97A0-ED8560D70318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6AABD8-06C1-49A4-B7D0-C73F47B6DF08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{59B733E0-D555-495B-93A0-705B2FB4D176}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{59B733E0-D555-495B-93A0-705B2FB4D176}"/>
   </bookViews>
   <sheets>
     <sheet name="kota" sheetId="5" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="166">
   <si>
     <t>b. Kepadatan Bangunan</t>
   </si>
@@ -126,30 +126,18 @@
     <t>kota</t>
   </si>
   <si>
-    <t>pekalongan</t>
-  </si>
-  <si>
     <t>provinsi</t>
   </si>
   <si>
-    <t>jawa tengah</t>
-  </si>
-  <si>
     <t>sk</t>
   </si>
   <si>
     <t>SK Nomor 430/1131 Tahun 2020</t>
   </si>
   <si>
-    <t>lokasi</t>
-  </si>
-  <si>
     <t xml:space="preserve"> id</t>
   </si>
   <si>
-    <t xml:space="preserve">astaga </t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -162,9 +150,6 @@
     <t>rt-rw</t>
   </si>
   <si>
-    <t>pekalongan barat</t>
-  </si>
-  <si>
     <t>tahun</t>
   </si>
   <si>
@@ -577,6 +562,15 @@
   </si>
   <si>
     <t>Jalan Aspal Hotmix</t>
+  </si>
+  <si>
+    <t>Pekalongan</t>
+  </si>
+  <si>
+    <t>Jawa tengah</t>
+  </si>
+  <si>
+    <t>Pekalongan Barat</t>
   </si>
 </sst>
 </file>
@@ -1245,10 +1239,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5192FDF1-76FA-4578-80AB-2E4CA55B23E3}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,38 +1254,32 @@
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>16</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>163</v>
       </c>
       <c r="C2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1305,7 +1293,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,37 +1313,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="K1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1363,10 +1351,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>165</v>
       </c>
       <c r="D2">
         <v>8</v>
@@ -1420,34 +1408,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" t="s">
         <v>96</v>
       </c>
-      <c r="D1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H1" t="s">
-        <v>101</v>
-      </c>
       <c r="I1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="J1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1716,9 +1704,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:BJ37"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AP1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AV17" sqref="AV17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1776,190 +1764,190 @@
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>77</v>
+      </c>
+      <c r="R1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>41</v>
       </c>
-      <c r="J1" t="s">
+      <c r="U1" t="s">
+        <v>78</v>
+      </c>
+      <c r="V1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB1" t="s">
         <v>80</v>
       </c>
-      <c r="K1" t="s">
+      <c r="AC1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK1" t="s">
         <v>47</v>
       </c>
-      <c r="L1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" t="s">
-        <v>81</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="AL1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR1" t="s">
         <v>50</v>
       </c>
-      <c r="P1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>82</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="AS1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AY1" t="s">
         <v>53</v>
       </c>
-      <c r="S1" t="s">
-        <v>54</v>
-      </c>
-      <c r="T1" t="s">
-        <v>46</v>
-      </c>
-      <c r="U1" t="s">
-        <v>83</v>
-      </c>
-      <c r="V1" t="s">
+      <c r="AZ1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BF1" t="s">
         <v>56</v>
       </c>
-      <c r="W1" t="s">
-        <v>57</v>
-      </c>
-      <c r="X1" t="s">
-        <v>84</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>92</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>76</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>77</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>93</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>79</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>61</v>
-      </c>
       <c r="BG1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="BH1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="BI1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="BJ1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.25">
@@ -2141,7 +2129,7 @@
         <v>16</v>
       </c>
       <c r="BH2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BI2">
         <v>0.22675162072980901</v>
@@ -2329,7 +2317,7 @@
         <v>16</v>
       </c>
       <c r="BH3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BI3">
         <v>0.22675162072980901</v>
@@ -2517,7 +2505,7 @@
         <v>14</v>
       </c>
       <c r="BH4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="BI4">
         <v>0.24186464667639004</v>
@@ -2705,7 +2693,7 @@
         <v>14</v>
       </c>
       <c r="BH5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="BI5">
         <v>0.24186464667639004</v>
@@ -2715,6 +2703,9 @@
       </c>
     </row>
     <row r="6" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
       <c r="B6">
         <v>1</v>
       </c>
@@ -2890,7 +2881,7 @@
         <v>11</v>
       </c>
       <c r="BH6" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="BI6">
         <v>0.20247790542534189</v>
@@ -2910,7 +2901,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:BK52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L53" sqref="L53"/>
     </sheetView>
@@ -2970,193 +2961,193 @@
   <sheetData>
     <row r="1" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" t="s">
-        <v>31</v>
-      </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" t="s">
         <v>40</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" t="s">
+        <v>77</v>
+      </c>
+      <c r="S1" t="s">
+        <v>48</v>
+      </c>
+      <c r="T1" t="s">
+        <v>49</v>
+      </c>
+      <c r="U1" t="s">
         <v>41</v>
       </c>
-      <c r="K1" t="s">
+      <c r="V1" t="s">
+        <v>78</v>
+      </c>
+      <c r="W1" t="s">
+        <v>51</v>
+      </c>
+      <c r="X1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC1" t="s">
         <v>80</v>
       </c>
-      <c r="L1" t="s">
+      <c r="AD1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1" t="s">
-        <v>81</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="AM1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS1" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" t="s">
-        <v>51</v>
-      </c>
-      <c r="R1" t="s">
-        <v>82</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="AT1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ1" t="s">
         <v>53</v>
       </c>
-      <c r="T1" t="s">
-        <v>54</v>
-      </c>
-      <c r="U1" t="s">
-        <v>46</v>
-      </c>
-      <c r="V1" t="s">
-        <v>83</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="BA1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BG1" t="s">
         <v>56</v>
       </c>
-      <c r="X1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>92</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>76</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>77</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>93</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>79</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>61</v>
-      </c>
       <c r="BH1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="BI1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="BJ1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="BK1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:63" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3341,7 +3332,7 @@
         <v>19</v>
       </c>
       <c r="BI2" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ2" s="5">
         <v>0.24460317460317457</v>
@@ -3532,7 +3523,7 @@
         <v>18</v>
       </c>
       <c r="BI3" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ3" s="5">
         <v>0.20619282195636873</v>
@@ -3723,7 +3714,7 @@
         <v>16</v>
       </c>
       <c r="BI4" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ4" s="5">
         <v>0.20764119601328904</v>
@@ -3914,7 +3905,7 @@
         <v>22</v>
       </c>
       <c r="BI5" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ5" s="5">
         <v>0.31194704175761007</v>
@@ -4105,7 +4096,7 @@
         <v>23</v>
       </c>
       <c r="BI6" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ6" s="5">
         <v>0.32470355731225303</v>
@@ -4296,7 +4287,7 @@
         <v>22</v>
       </c>
       <c r="BI7" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ7" s="5">
         <v>0.28693031118421208</v>
@@ -4487,7 +4478,7 @@
         <v>17</v>
       </c>
       <c r="BI8" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ8" s="5">
         <v>0.22004975736639551</v>
@@ -4678,7 +4669,7 @@
         <v>18</v>
       </c>
       <c r="BI9" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ9" s="5">
         <v>0.27636197336077289</v>
@@ -4869,7 +4860,7 @@
         <v>19</v>
       </c>
       <c r="BI10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ10">
         <v>0.24460317460317457</v>
@@ -5060,7 +5051,7 @@
         <v>18</v>
       </c>
       <c r="BI11" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ11">
         <v>0.20619282195636873</v>
@@ -5251,7 +5242,7 @@
         <v>16</v>
       </c>
       <c r="BI12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ12">
         <v>0.20764119601328904</v>
@@ -5442,7 +5433,7 @@
         <v>22</v>
       </c>
       <c r="BI13" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ13">
         <v>0.31194704175761007</v>
@@ -5633,7 +5624,7 @@
         <v>23</v>
       </c>
       <c r="BI14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ14">
         <v>0.32470355731225303</v>
@@ -5824,7 +5815,7 @@
         <v>22</v>
       </c>
       <c r="BI15" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ15">
         <v>0.28693031118421208</v>
@@ -6015,7 +6006,7 @@
         <v>17</v>
       </c>
       <c r="BI16" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ16">
         <v>0.22004975736639551</v>
@@ -6206,7 +6197,7 @@
         <v>18</v>
       </c>
       <c r="BI17" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ17">
         <v>0.27636197336077289</v>
@@ -6397,7 +6388,7 @@
         <v>14</v>
       </c>
       <c r="BI18" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="BJ18" s="4">
         <v>0.18031746031746035</v>
@@ -6588,7 +6579,7 @@
         <v>18</v>
       </c>
       <c r="BI19" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ19" s="4">
         <v>0.21296459413173868</v>
@@ -6779,7 +6770,7 @@
         <v>16</v>
       </c>
       <c r="BI20" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ20" s="4">
         <v>0.21096345514950166</v>
@@ -6970,7 +6961,7 @@
         <v>21</v>
       </c>
       <c r="BI21" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ21" s="4">
         <v>0.29390942428391309</v>
@@ -7161,7 +7152,7 @@
         <v>23</v>
       </c>
       <c r="BI22" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ22" s="4">
         <v>0.32068096505242327</v>
@@ -7352,7 +7343,7 @@
         <v>22</v>
       </c>
       <c r="BI23" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ23" s="4">
         <v>0.27162418873523247</v>
@@ -7543,7 +7534,7 @@
         <v>17</v>
       </c>
       <c r="BI24" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ24" s="4">
         <v>0.23809943317432028</v>
@@ -7734,7 +7725,7 @@
         <v>15</v>
       </c>
       <c r="BI25" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="BJ25" s="4">
         <v>0.24045901659803509</v>
@@ -7925,7 +7916,7 @@
         <v>14</v>
       </c>
       <c r="BI26" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="BJ26">
         <v>0.18031746031746035</v>
@@ -8116,7 +8107,7 @@
         <v>18</v>
       </c>
       <c r="BI27" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ27">
         <v>0.21296459413173868</v>
@@ -8307,7 +8298,7 @@
         <v>16</v>
       </c>
       <c r="BI28" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ28">
         <v>0.21096345514950166</v>
@@ -8498,7 +8489,7 @@
         <v>21</v>
       </c>
       <c r="BI29" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ29">
         <v>0.29390942428391309</v>
@@ -8689,7 +8680,7 @@
         <v>23</v>
       </c>
       <c r="BI30" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ30">
         <v>0.32068096505242327</v>
@@ -8880,7 +8871,7 @@
         <v>22</v>
       </c>
       <c r="BI31" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ31">
         <v>0.27162418873523247</v>
@@ -9071,7 +9062,7 @@
         <v>17</v>
       </c>
       <c r="BI32" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ32">
         <v>0.23809943317432028</v>
@@ -9262,7 +9253,7 @@
         <v>15</v>
       </c>
       <c r="BI33" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="BJ33">
         <v>0.24045901659803509</v>
@@ -9453,7 +9444,7 @@
         <v>14</v>
       </c>
       <c r="BI34" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="BJ34">
         <v>0.18031746031746035</v>
@@ -9644,7 +9635,7 @@
         <v>18</v>
       </c>
       <c r="BI35" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ35">
         <v>0.21296459413173868</v>
@@ -9835,7 +9826,7 @@
         <v>16</v>
       </c>
       <c r="BI36" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ36">
         <v>0.21096345514950166</v>
@@ -10026,7 +10017,7 @@
         <v>21</v>
       </c>
       <c r="BI37" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ37">
         <v>0.29390942428391309</v>
@@ -10217,7 +10208,7 @@
         <v>13</v>
       </c>
       <c r="BI38" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="BJ38">
         <v>0.18107057544203364</v>
@@ -10408,7 +10399,7 @@
         <v>22</v>
       </c>
       <c r="BI39" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ39">
         <v>0.27162418873523247</v>
@@ -10599,7 +10590,7 @@
         <v>17</v>
       </c>
       <c r="BI40" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BJ40">
         <v>0.23809943317432028</v>
@@ -10790,7 +10781,7 @@
         <v>15</v>
       </c>
       <c r="BI41" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="BJ41">
         <v>0.24045901659803509</v>
@@ -10904,31 +10895,31 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
       <c r="C1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="G1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="H1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="I1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -10945,13 +10936,13 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F2">
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="K2" s="1"/>
     </row>
@@ -10969,13 +10960,13 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F3">
         <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -10993,13 +10984,13 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F4">
         <v>39</v>
       </c>
       <c r="G4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -11017,13 +11008,13 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F5">
         <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="K5" s="1"/>
     </row>
@@ -11041,13 +11032,13 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F6">
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="K6" s="1"/>
     </row>
@@ -11065,13 +11056,13 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F7">
         <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="K7" s="1"/>
     </row>
@@ -11089,13 +11080,13 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F8">
         <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="K8" s="1"/>
     </row>
@@ -11113,13 +11104,13 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F9">
         <v>3</v>
       </c>
       <c r="G9" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="K9" s="1"/>
     </row>
@@ -11137,13 +11128,13 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F10">
         <v>50</v>
       </c>
       <c r="G10" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -11160,13 +11151,13 @@
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F11">
         <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -11183,13 +11174,13 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F12">
         <v>50</v>
       </c>
       <c r="G12" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -11206,16 +11197,16 @@
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F13">
         <v>217</v>
       </c>
       <c r="G13" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="H13" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="I13">
         <v>180000000</v>
@@ -11235,16 +11226,16 @@
         <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F14">
         <v>150</v>
       </c>
       <c r="G14" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="H14" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="I14">
         <v>135000000</v>
@@ -11264,16 +11255,16 @@
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F15">
         <v>38</v>
       </c>
       <c r="G15" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H15" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="I15">
         <v>45000000</v>
@@ -11293,19 +11284,19 @@
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F16">
         <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H16" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="I16" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="11:15" x14ac:dyDescent="0.25">
@@ -11316,10 +11307,10 @@
         <v>1</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="O19" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="11:15" x14ac:dyDescent="0.25">
@@ -11330,10 +11321,10 @@
         <v>2</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="O20" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="11:15" x14ac:dyDescent="0.25">
@@ -11344,10 +11335,10 @@
         <v>3</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="O21" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="11:15" x14ac:dyDescent="0.25">
@@ -11358,10 +11349,10 @@
         <v>4</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="O22" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="11:15" x14ac:dyDescent="0.25">
@@ -11372,10 +11363,10 @@
         <v>5</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="O23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="11:15" x14ac:dyDescent="0.25">
@@ -11386,10 +11377,10 @@
         <v>6</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="O24" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="11:15" x14ac:dyDescent="0.25">
@@ -11400,10 +11391,10 @@
         <v>7</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="O25" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="11:15" x14ac:dyDescent="0.25">
@@ -11414,74 +11405,74 @@
         <v>8</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="O26" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="11:15" x14ac:dyDescent="0.25">
       <c r="N27" s="3" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="O27" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="11:15" x14ac:dyDescent="0.25">
       <c r="N28" s="3" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="O28" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="11:15" x14ac:dyDescent="0.25">
       <c r="N29" s="3" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="O29" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="11:15" x14ac:dyDescent="0.25">
       <c r="N30" s="3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="O30" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="11:15" x14ac:dyDescent="0.25">
       <c r="N31" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="O31" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="11:15" x14ac:dyDescent="0.25">
       <c r="N32" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="O32" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N33" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="O33" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N34" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="O34" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -11513,28 +11504,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -11542,7 +11533,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E2" t="str">
         <f>CONCATENATE(F2,G2)</f>
@@ -11552,13 +11543,13 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -11566,7 +11557,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E17" si="0">CONCATENATE(F3,G3)</f>
@@ -11576,13 +11567,13 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -11590,7 +11581,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -11600,13 +11591,13 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -11614,7 +11605,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -11624,13 +11615,13 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -11638,7 +11629,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -11648,13 +11639,13 @@
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -11662,7 +11653,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -11672,13 +11663,13 @@
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -11686,7 +11677,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -11696,13 +11687,13 @@
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -11714,13 +11705,13 @@
         <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -11732,13 +11723,13 @@
         <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -11750,13 +11741,13 @@
         <v>4</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -11768,13 +11759,13 @@
         <v>5</v>
       </c>
       <c r="G12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -11786,13 +11777,13 @@
         <v>5</v>
       </c>
       <c r="G13" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -11804,13 +11795,13 @@
         <v>6</v>
       </c>
       <c r="G14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -11822,13 +11813,13 @@
         <v>6</v>
       </c>
       <c r="G15" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -11840,13 +11831,13 @@
         <v>7</v>
       </c>
       <c r="G16" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="5:9" x14ac:dyDescent="0.25">
@@ -11858,13 +11849,13 @@
         <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="5:9" x14ac:dyDescent="0.25">

</xml_diff>